<commit_message>
Correcting a bug in FossilELC_Trans (ACT was written as ATC: which induced to warnings causing the the GAMS engine to stop)
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_FossilELC_Trans.xlsx
+++ b/SubRes_Tmpl/SubRES_FossilELC_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\Veda_models\IEMM_v60_10-1-master\SubRes_Tmpl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SubRes_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B947B03A-3980-4F4A-95E1-9D840BE3E169}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493019B2-4A35-4B5C-8E7E-FF606BDA9B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9435" yWindow="-17400" windowWidth="30960" windowHeight="16920" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3876" yWindow="-14184" windowWidth="17280" windowHeight="10044" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="23" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="511">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -1652,9 +1652,6 @@
   </si>
   <si>
     <t>EN_STG_PHS</t>
-  </si>
-  <si>
-    <t>ATC</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2032,7 @@
     <cellStyle name="Header: top rows" xfId="42" xr:uid="{FD1E3697-CB45-485F-BB56-B65C12748072}"/>
     <cellStyle name="Heading1" xfId="43" xr:uid="{9482AD06-2649-43BC-9C2B-EAB330365766}"/>
     <cellStyle name="Heading2" xfId="44" xr:uid="{E878A1AA-6E44-4F76-AC54-1A77211EC199}"/>
-    <cellStyle name="Neutre" xfId="53" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="53" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="31" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 11 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -2092,7 +2089,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2418,7 +2415,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
@@ -2464,12 +2461,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
@@ -2482,7 +2479,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="15" thickBot="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5643,14 +5640,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="35" width="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="4.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21">
@@ -7778,12 +7775,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="34" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="34" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:216">
@@ -37205,17 +37202,17 @@
   <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11">
@@ -37330,9 +37327,9 @@
         <v>510</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>511</v>
-      </c>
-      <c r="G9" s="11">
+        <v>35</v>
+      </c>
+      <c r="G9" s="12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Coal IGCC and Gas CC retrofit possibilities
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_FossilELC_Trans.xlsx
+++ b/SubRes_Tmpl/SubRES_FossilELC_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SubRes_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3091CC-6957-443F-913A-133BECF84E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9449CBD-832E-445F-BBE9-84440B52918D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3672" yWindow="-17388" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12072" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="23" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="522">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -1702,6 +1702,15 @@
   </si>
   <si>
     <t>-ELCNUC</t>
+  </si>
+  <si>
+    <t>EN_Z*</t>
+  </si>
+  <si>
+    <t>-CAPTURE_*</t>
+  </si>
+  <si>
+    <t>-EN_Z*,-CAPTURE_*</t>
   </si>
 </sst>
 </file>
@@ -1730,7 +1739,7 @@
     <numFmt numFmtId="181" formatCode="\Te\x\t"/>
     <numFmt numFmtId="182" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="70">
+  <fonts count="64">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2135,50 +2144,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="54"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="49"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color indexed="54"/>
-      <name val="Calibri Light"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2410,7 +2378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -2741,100 +2709,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="dashed">
-        <color indexed="55"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="49"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="49"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="9"/>
-      </left>
-      <right style="thick">
-        <color indexed="9"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="55"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="44"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="44"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="55"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="49"/>
       </top>
       <bottom style="dashed">
         <color indexed="55"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="49"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="55"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="49"/>
-      </top>
-      <bottom style="double">
-        <color indexed="49"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5863,7 +5742,7 @@
     <xf numFmtId="0" fontId="2" fillId="42" borderId="9">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="36" applyNumberFormat="0" applyFont="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="29" applyNumberFormat="0" applyFont="0" applyFill="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -5877,7 +5756,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -44161,7 +44040,7 @@
   <dimension ref="B1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -44222,6 +44101,9 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
+      <c r="E4" s="16" t="s">
+        <v>520</v>
+      </c>
       <c r="G4">
         <v>1</v>
       </c>
@@ -44244,6 +44126,9 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
+      <c r="E6" s="16" t="s">
+        <v>520</v>
+      </c>
       <c r="G6" s="5">
         <f>31.536/1.055</f>
         <v>29.891943127962087</v>
@@ -44273,26 +44158,41 @@
       <c r="D8" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="E8" s="16" t="s">
+        <v>521</v>
+      </c>
       <c r="G8" s="13">
-        <f>MAX(K2:K6)+1</f>
-        <v>2019</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="9" spans="2:11" s="11" customFormat="1">
       <c r="B9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="G9" s="11">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" s="11" customFormat="1">
+      <c r="B10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G10" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:11" s="11" customFormat="1"/>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Adding PtL and BtL to the model & correcting hydrogen costs
</commit_message>
<xml_diff>
--- a/SubRes_Tmpl/SubRES_FossilELC_Trans.xlsx
+++ b/SubRes_Tmpl/SubRES_FossilELC_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SubRes_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9449CBD-832E-445F-BBE9-84440B52918D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C125B8-08C8-4A99-8749-D78E3637CBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12072" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41625" yWindow="4530" windowWidth="23040" windowHeight="12120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="23" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="523">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -1711,6 +1711,9 @@
   </si>
   <si>
     <t>-EN_Z*,-CAPTURE_*</t>
+  </si>
+  <si>
+    <t>Deactivated~TFM_INS</t>
   </si>
 </sst>
 </file>
@@ -44040,7 +44043,7 @@
   <dimension ref="B1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -44228,7 +44231,7 @@
     </row>
     <row r="21" spans="2:14">
       <c r="B21" s="18" t="s">
-        <v>6</v>
+        <v>522</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>

</xml_diff>